<commit_message>
maven jenkins and randmon number generatioon fix
</commit_message>
<xml_diff>
--- a/src/test/resources/config/config.xml.xlsx
+++ b/src/test/resources/config/config.xml.xlsx
@@ -11,7 +11,6 @@
     <sheet name="TempList" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -394,7 +393,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -426,20 +425,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
@@ -447,6 +446,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -456,7 +458,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -465,7 +467,7 @@
     <col min="5" max="5" width="41.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>2</v>
       </c>
@@ -485,7 +487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>

</xml_diff>